<commit_message>
mise en place de la traduction
</commit_message>
<xml_diff>
--- a/src/assets/translation_orderboard.xlsx
+++ b/src/assets/translation_orderboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\www\orderBoard\front\board\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C873AAE2-D8DC-4237-8032-A1281A64D9F5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE8FC43-812B-41B5-B572-4D95BF883C0C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,15 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>FR</t>
-  </si>
-  <si>
-    <t>EN</t>
-  </si>
-  <si>
-    <t>KEY</t>
-  </si>
-  <si>
     <t>TEST</t>
   </si>
   <si>
@@ -43,6 +34,15 @@
   </si>
   <si>
     <t>that a test</t>
+  </si>
+  <si>
+    <t>fr</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>key</t>
   </si>
 </sst>
 </file>
@@ -370,7 +370,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -381,24 +381,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
un peu de traduction
</commit_message>
<xml_diff>
--- a/src/assets/translation_orderboard.xlsx
+++ b/src/assets/translation_orderboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\www\orderBoard\front\board\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65FDBD7-2FF4-4FE5-8D30-45E97DA2546A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85889A5A-8FDE-486E-88AF-1011A7420948}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>fr</t>
   </si>
@@ -130,6 +130,21 @@
   </si>
   <si>
     <t>Connexion</t>
+  </si>
+  <si>
+    <t>Vendeurs</t>
+  </si>
+  <si>
+    <t>Sellers</t>
+  </si>
+  <si>
+    <t>USERS.TITLE</t>
+  </si>
+  <si>
+    <t>Liste des vendeurs</t>
+  </si>
+  <si>
+    <t>MENU.USERS</t>
   </si>
 </sst>
 </file>
@@ -454,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -610,6 +625,28 @@
         <v>23</v>
       </c>
     </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ajout page contact vierge
</commit_message>
<xml_diff>
--- a/src/assets/translation_orderboard.xlsx
+++ b/src/assets/translation_orderboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\www\orderBoard\front\board\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962732A3-FE34-4AAD-B11C-86EFA1B2C8BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771035BE-2394-4BAF-826E-F2BC296A74A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>fr</t>
   </si>
@@ -163,6 +163,15 @@
   </si>
   <si>
     <t>Continue</t>
+  </si>
+  <si>
+    <t>CONTACT_BOX.CONTACT_US</t>
+  </si>
+  <si>
+    <t>Contact / Aide</t>
+  </si>
+  <si>
+    <t>Contact / Help</t>
   </si>
 </sst>
 </file>
@@ -487,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -687,6 +696,17 @@
         <v>45</v>
       </c>
     </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
formulaire avec recuperation user au login
</commit_message>
<xml_diff>
--- a/src/assets/translation_orderboard.xlsx
+++ b/src/assets/translation_orderboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\www\orderBoard\front\board\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771035BE-2394-4BAF-826E-F2BC296A74A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA19CC5B-9619-4BC0-A077-69305F97B17A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="87">
   <si>
     <t>fr</t>
   </si>
@@ -172,6 +172,120 @@
   </si>
   <si>
     <t>Contact / Help</t>
+  </si>
+  <si>
+    <t>CONTACT.INPUT_EMPTY</t>
+  </si>
+  <si>
+    <t>CONTACT.EMAIL_UNVALID</t>
+  </si>
+  <si>
+    <t>Email non valide</t>
+  </si>
+  <si>
+    <t>Email unvalid</t>
+  </si>
+  <si>
+    <t>CONTACT.TITLE</t>
+  </si>
+  <si>
+    <t>CONTACT.SUPPORT_MESSAGE</t>
+  </si>
+  <si>
+    <t>CONTACT.ADMIN_MESSAGE</t>
+  </si>
+  <si>
+    <t>CONTACT.SUPPORT_TITLE</t>
+  </si>
+  <si>
+    <t>CONTACT.ADMIN_TITLE</t>
+  </si>
+  <si>
+    <t>Vous rencontrez un problème technique lié à l'application.</t>
+  </si>
+  <si>
+    <t>You have a technical problem with the application.</t>
+  </si>
+  <si>
+    <t>Contacter le support</t>
+  </si>
+  <si>
+    <t>Contact support</t>
+  </si>
+  <si>
+    <t>You have a functional problem.</t>
+  </si>
+  <si>
+    <t>Vous rencontrez un problème fonctionnel.</t>
+  </si>
+  <si>
+    <t>Contacter un administrateur</t>
+  </si>
+  <si>
+    <t>Contact an administrator</t>
+  </si>
+  <si>
+    <t>CONTACT.BACK_BUTTON</t>
+  </si>
+  <si>
+    <t>CONTACT.INPUT_LOGIN</t>
+  </si>
+  <si>
+    <t>CONTACT.INPUT_NAME</t>
+  </si>
+  <si>
+    <t>CONTACT.INPUT_EMAIL</t>
+  </si>
+  <si>
+    <t>CONTACT.INPUT_FIRSTNAME</t>
+  </si>
+  <si>
+    <t>CONTACT.INPUT_PHONE</t>
+  </si>
+  <si>
+    <t>CONTACT.INPUT_MESSAGE</t>
+  </si>
+  <si>
+    <t>CONTACT.INPUT_SUBMIT</t>
+  </si>
+  <si>
+    <t>Retour</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Firstname</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>Prénom</t>
+  </si>
+  <si>
+    <t>Téléphone (optionnel)</t>
+  </si>
+  <si>
+    <t>Phone (optionnal)</t>
+  </si>
+  <si>
+    <t>Envoyer</t>
+  </si>
+  <si>
+    <t>Send</t>
+  </si>
+  <si>
+    <t>Message (300 caractères)</t>
+  </si>
+  <si>
+    <t>Message (300 characters)</t>
   </si>
 </sst>
 </file>
@@ -496,16 +610,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.08984375" customWidth="1"/>
-    <col min="2" max="2" width="25.54296875" customWidth="1"/>
+    <col min="1" max="1" width="31.36328125" customWidth="1"/>
+    <col min="2" max="2" width="49.54296875" customWidth="1"/>
     <col min="3" max="3" width="20.7265625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -707,6 +821,171 @@
         <v>48</v>
       </c>
     </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" t="s">
+        <v>81</v>
+      </c>
+      <c r="C31" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ajout param shop au user
</commit_message>
<xml_diff>
--- a/src/assets/translation_orderboard.xlsx
+++ b/src/assets/translation_orderboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\www\orderBoard\front\board\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA19CC5B-9619-4BC0-A077-69305F97B17A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F004F2-A859-422A-81FE-3567EA99F43C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="90">
   <si>
     <t>fr</t>
   </si>
@@ -286,6 +286,15 @@
   </si>
   <si>
     <t>Message (300 characters)</t>
+  </si>
+  <si>
+    <t>CONTACT.INPUT_SHOP</t>
+  </si>
+  <si>
+    <t>Magasin</t>
+  </si>
+  <si>
+    <t>Shop</t>
   </si>
 </sst>
 </file>
@@ -610,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -986,6 +995,17 @@
         <v>84</v>
       </c>
     </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>